<commit_message>
first working alpha version
</commit_message>
<xml_diff>
--- a/jps_maze/src/jps_maze/res/board_creator.xlsx
+++ b/jps_maze/src/jps_maze/res/board_creator.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\root\INTP-ros\jps_maze\src\jps_maze\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F8BA095-952F-4727-82D1-D18654419EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9272FFE4-7FCC-4158-9517-61D3588918EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="6135" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="33720" yWindow="6135" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="board1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,24 +549,11 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -595,6 +582,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -613,9 +603,19 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="4"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -928,11 +928,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BW19" sqref="BW19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S62" sqref="S62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1002,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="V1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W1">
         <v>0</v>
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="BC1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD1">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -1295,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="BC2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD2">
         <v>0</v>
@@ -1390,7 +1390,7 @@
         <v>1</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="BC3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD3">
         <v>0</v>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="BC4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD4">
         <v>0</v>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -1877,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="BC5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD5">
         <v>0</v>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -2166,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -11424,10 +11424,10 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -11618,7 +11618,7 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -11812,7 +11812,7 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -12006,7 +12006,7 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -12033,7 +12033,7 @@
         <v>0</v>
       </c>
       <c r="N58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -12048,7 +12048,7 @@
         <v>0</v>
       </c>
       <c r="S58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T58">
         <v>0</v>
@@ -12200,7 +12200,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -12227,7 +12227,7 @@
         <v>0</v>
       </c>
       <c r="N59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O59">
         <v>0</v>
@@ -12242,7 +12242,7 @@
         <v>0</v>
       </c>
       <c r="S59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T59">
         <v>0</v>
@@ -12394,7 +12394,7 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -12421,7 +12421,7 @@
         <v>0</v>
       </c>
       <c r="N60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O60">
         <v>0</v>
@@ -12436,7 +12436,7 @@
         <v>0</v>
       </c>
       <c r="S60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T60">
         <v>0</v>
@@ -12550,7 +12550,7 @@
         <v>0</v>
       </c>
       <c r="BE60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF60">
         <v>0</v>
@@ -12615,7 +12615,7 @@
         <v>0</v>
       </c>
       <c r="N61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61">
         <v>0</v>
@@ -12630,7 +12630,7 @@
         <v>0</v>
       </c>
       <c r="S61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T61">
         <v>0</v>
@@ -12744,7 +12744,7 @@
         <v>0</v>
       </c>
       <c r="BE61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF61">
         <v>0</v>
@@ -13176,7 +13176,7 @@
         <v>0</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -13352,22 +13352,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:BL64">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixing error in board
</commit_message>
<xml_diff>
--- a/jps_maze/src/jps_maze/res/board_creator.xlsx
+++ b/jps_maze/src/jps_maze/res/board_creator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\root\INTP-ros\jps_maze\src\jps_maze\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDA232C-3E04-44A3-AFF6-648BB7DE022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9487F280-1840-4E0B-BEF0-E3942066D4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="6135" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="board1" sheetId="1" r:id="rId1"/>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X54" sqref="X54"/>
+    <sheetView tabSelected="1" zoomScale="29" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BL64" sqref="A1:BL64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6312,6 +6312,9 @@
         <v>0</v>
       </c>
       <c r="AT28">
+        <v>0</v>
+      </c>
+      <c r="AU28">
         <v>0</v>
       </c>
       <c r="AV28">

</xml_diff>